<commit_message>
add new table workarea
</commit_message>
<xml_diff>
--- a/Document/DB design.xlsx
+++ b/Document/DB design.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0227B0D-DA92-4B6E-9BD5-FF6EECB17C10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DF644E-B593-42B7-B053-5E782FD7B231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="996" firstSheet="9" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="996" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Polygon_background" sheetId="13" r:id="rId1"/>
@@ -22,19 +22,20 @@
     <sheet name="fence_detain" sheetId="24" r:id="rId12"/>
     <sheet name="fence_danger" sheetId="27" r:id="rId13"/>
     <sheet name="fence_work" sheetId="30" r:id="rId14"/>
-    <sheet name="fence_fourcolor" sheetId="31" r:id="rId15"/>
-    <sheet name="fence_configpot" sheetId="33" r:id="rId16"/>
-    <sheet name="fence_configarea" sheetId="34" r:id="rId17"/>
-    <sheet name="inspection_point" sheetId="25" r:id="rId18"/>
-    <sheet name="asset_init_locate（bison）" sheetId="16" r:id="rId19"/>
-    <sheet name="camera Info（bison）" sheetId="18" r:id="rId20"/>
-    <sheet name="attendance fence（bison）" sheetId="17" r:id="rId21"/>
-    <sheet name="region（bison）" sheetId="20" r:id="rId22"/>
-    <sheet name="detain（bison）" sheetId="21" r:id="rId23"/>
-    <sheet name="danger（bison）" sheetId="22" r:id="rId24"/>
-    <sheet name="poi collection（网页）" sheetId="12" r:id="rId25"/>
-    <sheet name="electronic fence（网页）" sheetId="15" r:id="rId26"/>
-    <sheet name="变更履历" sheetId="14" r:id="rId27"/>
+    <sheet name="fence_workarea" sheetId="35" r:id="rId15"/>
+    <sheet name="fence_fourcolor" sheetId="31" r:id="rId16"/>
+    <sheet name="fence_configpot" sheetId="33" r:id="rId17"/>
+    <sheet name="fence_configarea" sheetId="34" r:id="rId18"/>
+    <sheet name="inspection_point" sheetId="25" r:id="rId19"/>
+    <sheet name="asset_init_locate（bison）" sheetId="16" r:id="rId20"/>
+    <sheet name="camera Info（bison）" sheetId="18" r:id="rId21"/>
+    <sheet name="attendance fence（bison）" sheetId="17" r:id="rId22"/>
+    <sheet name="region（bison）" sheetId="20" r:id="rId23"/>
+    <sheet name="detain（bison）" sheetId="21" r:id="rId24"/>
+    <sheet name="danger（bison）" sheetId="22" r:id="rId25"/>
+    <sheet name="poi collection（网页）" sheetId="12" r:id="rId26"/>
+    <sheet name="electronic fence（网页）" sheetId="15" r:id="rId27"/>
+    <sheet name="变更履历" sheetId="14" r:id="rId28"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="385">
   <si>
     <t>文字列</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1665,6 +1666,29 @@
   </si>
   <si>
     <t>id，唯一，必须</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v1.2.4</t>
+  </si>
+  <si>
+    <t>fence_workarea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>化工厂增加作业管理区域表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置-作业管理区域用表（化工厂用）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表名：fence_workarea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>报警检测开关</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6474,6 +6498,708 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8159C008-51A2-4AF6-9453-F9D3695C902F}">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="B1:K47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="35"/>
+    <col min="3" max="3" width="14.625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="35" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="35" customWidth="1"/>
+    <col min="6" max="6" width="31.125" style="35" customWidth="1"/>
+    <col min="7" max="16384" width="8.875" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="36"/>
+      <c r="C3" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+    </row>
+    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="36"/>
+      <c r="C6" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="36"/>
+      <c r="C7" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>378</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="36"/>
+      <c r="C8" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+    </row>
+    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="36"/>
+      <c r="C10" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="36"/>
+      <c r="C11" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="12" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+      <c r="C18" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="36"/>
+      <c r="C20" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="36"/>
+      <c r="C23" s="52" t="s">
+        <v>383</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE683C6-7E88-4429-AA7F-55BEB8467DAB}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -7045,7 +7771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5184FEA4-C741-410C-87F8-2324908EA58C}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -7617,7 +8343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1522FF-6BF2-4B1A-BE23-61AF86B40C74}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -8191,14 +8917,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ADED41-395A-4A8F-8993-00A4449A299D}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -8760,681 +9486,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:K48"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20:M21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="0.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="1"/>
-    <col min="3" max="3" width="11.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10165,6 +10216,681 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B1:K48"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20:M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="1"/>
+    <col min="3" max="3" width="11.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F555419B-A5B4-40B5-8369-E068ACA90498}">
   <dimension ref="B1:K47"/>
   <sheetViews>
@@ -10819,7 +11545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B248F353-AF05-48D5-B0F8-000FF89FAE10}">
   <dimension ref="B1:K40"/>
   <sheetViews>
@@ -11384,7 +12110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D4992C-8FC3-407E-AB24-301E21E12784}">
   <dimension ref="B1:K38"/>
   <sheetViews>
@@ -11915,7 +12641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9B918E-F7F0-4225-8E2E-A870DF8C9BF9}">
   <dimension ref="B1:K39"/>
   <sheetViews>
@@ -12466,7 +13192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83408E44-36B6-4215-B050-13A2AF74066B}">
   <dimension ref="B1:K38"/>
   <sheetViews>
@@ -12997,7 +13723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:K45"/>
   <sheetViews>
@@ -13619,7 +14345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:K42"/>
   <sheetViews>
@@ -14224,13 +14950,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:G62"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14743,12 +15469,24 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="18"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="19"/>
+      <c r="B27" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>380</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F27" s="32">
+        <v>43944</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="18"/>

</xml_diff>